<commit_message>
correct ODK sheet 'options' -> 'choices'
</commit_message>
<xml_diff>
--- a/data/mortality_survey_simple_kobo.xlsx
+++ b/data/mortality_survey_simple_kobo.xlsx
@@ -1,493 +1,486 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbarks/OCA-training/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4138F263-FA30-B84B-AC49-18725252A569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33580" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="options" sheetId="2" r:id="rId2"/>
-    <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="153">
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>hint</t>
-  </si>
-  <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>relevant</t>
-  </si>
-  <si>
-    <t>repeat_count</t>
-  </si>
-  <si>
-    <t>calculation</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Date must be in July 2021</t>
-  </si>
-  <si>
-    <t>. &gt;=  date('07/01/2021') and . &lt;=  date('08/01/2021')</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>select_one ed3bh57</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>cluster</t>
-  </si>
-  <si>
-    <t>Cluster Number</t>
-  </si>
-  <si>
-    <t>Cluster number must be bless than 20</t>
-  </si>
-  <si>
-    <t>. &lt; 20</t>
-  </si>
-  <si>
-    <t>select_one it57u05</t>
-  </si>
-  <si>
-    <t>source_water</t>
-  </si>
-  <si>
-    <t>Where do take drinking water from?</t>
-  </si>
-  <si>
-    <t>${hh_present} = 'yes' and ${hh_consents} = 'yes'</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>source_water_other</t>
-  </si>
-  <si>
-    <t>Please, specify other source of water</t>
-  </si>
-  <si>
-    <t>${source_water} = 'other__specify'</t>
-  </si>
-  <si>
-    <t>select_one male_female</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>select_one yy4oh98</t>
-  </si>
-  <si>
-    <t>age_under_one</t>
-  </si>
-  <si>
-    <t>Is this household member aged less than 1 year?</t>
-  </si>
-  <si>
-    <t>age_months</t>
-  </si>
-  <si>
-    <t>Age in months</t>
-  </si>
-  <si>
-    <t>If months 12 or more enter age in years</t>
-  </si>
-  <si>
-    <t>. &lt; 12</t>
-  </si>
-  <si>
-    <t>${age_under_one} = 'yes'</t>
-  </si>
-  <si>
-    <t>age_years</t>
-  </si>
-  <si>
-    <t>Age in years</t>
-  </si>
-  <si>
-    <t>${age_under_one} = 'no'</t>
-  </si>
-  <si>
-    <t>select_one ap9tz70</t>
-  </si>
-  <si>
-    <t>illness</t>
-  </si>
-  <si>
-    <t>Did this household member experienced illness in the last 14 days?</t>
-  </si>
-  <si>
-    <t>${age_years} &lt; 5 or ${age_months} != ''</t>
-  </si>
-  <si>
-    <t>ilness_other</t>
-  </si>
-  <si>
-    <t>If other illness, specify, please</t>
-  </si>
-  <si>
-    <t>${illness} = 'other__specify'</t>
-  </si>
-  <si>
-    <t>select_one lj1vc50</t>
-  </si>
-  <si>
-    <t>oedema</t>
-  </si>
-  <si>
-    <t>Was oedema detected?</t>
-  </si>
-  <si>
-    <t>${age_months} &gt;= 6 or ${age_years} &lt; 5</t>
-  </si>
-  <si>
-    <t>muac</t>
-  </si>
-  <si>
-    <t>MUAC measurement</t>
-  </si>
-  <si>
-    <t>in mm</t>
-  </si>
-  <si>
-    <t>MUAC must be between 50 and 280 mm</t>
-  </si>
-  <si>
-    <t>. &gt; 50 and . &lt; 280</t>
-  </si>
-  <si>
-    <t>select_one nt2gp06</t>
-  </si>
-  <si>
-    <t>arrived</t>
-  </si>
-  <si>
-    <t>Did this household member arrive since the 15th of July 2020?</t>
-  </si>
-  <si>
-    <t>date_arrived</t>
-  </si>
-  <si>
-    <t>Date of arrival</t>
-  </si>
-  <si>
-    <t>Date has to be between July 2020 and August 2021</t>
-  </si>
-  <si>
-    <t>. &gt;=  date('07/01/2020') and . &lt;=  date('08/01/2021')</t>
-  </si>
-  <si>
-    <t>${arrived} = 'yes'</t>
-  </si>
-  <si>
-    <t>select_one uv39a86</t>
-  </si>
-  <si>
-    <t>departed</t>
-  </si>
-  <si>
-    <t>Did this household member depart since the 15th of July 2020?</t>
-  </si>
-  <si>
-    <t>date_departed</t>
-  </si>
-  <si>
-    <t>Date of departure</t>
-  </si>
-  <si>
-    <t>${departed} = 'yes'</t>
-  </si>
-  <si>
-    <t>select_one kk1ef13</t>
-  </si>
-  <si>
-    <t>born</t>
-  </si>
-  <si>
-    <t>Was this household member born since the 15th of July 2020?</t>
-  </si>
-  <si>
-    <t>date_born</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
-  <si>
-    <t>${born} = 'yes'</t>
-  </si>
-  <si>
-    <t>select_one died</t>
-  </si>
-  <si>
-    <t>died</t>
-  </si>
-  <si>
-    <t>Did this household member die since the 15th of July 2020?</t>
-  </si>
-  <si>
-    <t>date_died</t>
-  </si>
-  <si>
-    <t>Date of death</t>
-  </si>
-  <si>
-    <t>${died} = 'yes'</t>
-  </si>
-  <si>
-    <t>select_one kg73x52</t>
-  </si>
-  <si>
-    <t>cause_death</t>
-  </si>
-  <si>
-    <t>Cause of death</t>
-  </si>
-  <si>
-    <t>cause_death_other</t>
-  </si>
-  <si>
-    <t>If other cause of death, specify, please</t>
-  </si>
-  <si>
-    <t>${cause_death} = 'other__specify_'</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>ed3bh57</t>
-  </si>
-  <si>
-    <t>town_a</t>
-  </si>
-  <si>
-    <t>Town A</t>
-  </si>
-  <si>
-    <t>town_b</t>
-  </si>
-  <si>
-    <t>Town B</t>
-  </si>
-  <si>
-    <t>it57u05</t>
-  </si>
-  <si>
-    <t>city_water_network_piped_to_ho</t>
-  </si>
-  <si>
-    <t>City water network piped to household</t>
-  </si>
-  <si>
-    <t>tank_filled_by_a_truck_transpo</t>
-  </si>
-  <si>
-    <t>Tank filled by a truck transporting treated water</t>
-  </si>
-  <si>
-    <t>Tank filled by a truck transporting untreated water</t>
-  </si>
-  <si>
-    <t>direct_from_canal</t>
-  </si>
-  <si>
-    <t>Direct from canal</t>
-  </si>
-  <si>
-    <t>other__specify</t>
-  </si>
-  <si>
-    <t>Other (specify)</t>
-  </si>
-  <si>
-    <t>male_female</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>femal</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>yy4oh98</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>ap9tz70</t>
-  </si>
-  <si>
-    <t>yes__watery_diarrhoea</t>
-  </si>
-  <si>
-    <t>Yes, watery diarrhoea</t>
-  </si>
-  <si>
-    <t>yes__respiratory_infection</t>
-  </si>
-  <si>
-    <t>Yes, respiratory infection</t>
-  </si>
-  <si>
-    <t>yes__fever_and_rash</t>
-  </si>
-  <si>
-    <t>Yes, fever and rash</t>
-  </si>
-  <si>
-    <t>Yes, other (specify)</t>
-  </si>
-  <si>
-    <t>lj1vc50</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>nt2gp06</t>
-  </si>
-  <si>
-    <t>uv39a86</t>
-  </si>
-  <si>
-    <t>kk1ef13</t>
-  </si>
-  <si>
-    <t>kg73x52</t>
-  </si>
-  <si>
-    <t>diarrhoea</t>
-  </si>
-  <si>
-    <t>Diarrhoea</t>
-  </si>
-  <si>
-    <t>respiratory_infection</t>
-  </si>
-  <si>
-    <t>Respiratory infection</t>
-  </si>
-  <si>
-    <t>fever</t>
-  </si>
-  <si>
-    <t>Fever</t>
-  </si>
-  <si>
-    <t>during_pregnancy</t>
-  </si>
-  <si>
-    <t>During pregnancy</t>
-  </si>
-  <si>
-    <t>during_after_delivery__1_month</t>
-  </si>
-  <si>
-    <t>During/after delivery (&lt;1 month)</t>
-  </si>
-  <si>
-    <t>trauma_accident</t>
-  </si>
-  <si>
-    <t>Trauma/accident</t>
-  </si>
-  <si>
-    <t>violence</t>
-  </si>
-  <si>
-    <t>Violence</t>
-  </si>
-  <si>
-    <t>don_t_know</t>
-  </si>
-  <si>
-    <t>Don’t know</t>
-  </si>
-  <si>
-    <t>other__specify_</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>vYsUPjPAfLpLZEGZqSvzbR</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint_message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeat_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date must be in July 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. &gt;=  date('07/01/2021') and . &lt;=  date('08/01/2021')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one ed3bh57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster number must be bless than 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. &lt; 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one it57u05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where do take drinking water from?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${hh_present} = 'yes' and ${hh_consents} = 'yes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source_water_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please, specify other source of water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${source_water} = 'other__specify'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one male_female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one yy4oh98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_under_one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is this household member aged less than 1 year?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age in months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If months 12 or more enter age in years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. &lt; 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${age_under_one} = 'yes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age in years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${age_under_one} = 'no'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one ap9tz70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">illness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did this household member experienced illness in the last 14 days?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${age_years} &lt; 5 or ${age_months} != ''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ilness_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If other illness, specify, please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${illness} = 'other__specify'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one lj1vc50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oedema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was oedema detected?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${age_months} &gt;= 6 or ${age_years} &lt; 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUAC measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUAC must be between 50 and 280 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. &gt; 50 and . &lt; 280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one nt2gp06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrived</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did this household member arrive since the 15th of July 2020?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_arrived</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of arrival</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date has to be between July 2020 and August 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. &gt;=  date('07/01/2020') and . &lt;=  date('08/01/2021')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${arrived} = 'yes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one uv39a86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">departed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did this household member depart since the 15th of July 2020?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_departed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of departure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${departed} = 'yes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one kk1ef13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">born</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was this household member born since the 15th of July 2020?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_born</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${born} = 'yes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one died</t>
+  </si>
+  <si>
+    <t xml:space="preserve">died</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did this household member die since the 15th of July 2020?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_died</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${died} = 'yes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one kg73x52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cause_death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cause of death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cause_death_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If other cause of death, specify, please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${cause_death} = 'other__specify_'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ed3bh57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">town_a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Town A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">town_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Town B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it57u05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city_water_network_piped_to_ho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City water network piped to household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tank_filled_by_a_truck_transpo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tank filled by a truck transporting treated water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tank filled by a truck transporting untreated water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direct_from_canal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct from canal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other__specify</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other (specify)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male_female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">femal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yy4oh98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ap9tz70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes__watery_diarrhoea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, watery diarrhoea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes__respiratory_infection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, respiratory infection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes__fever_and_rash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, fever and rash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, other (specify)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lj1vc50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nt2gp06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uv39a86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kk1ef13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg73x52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diarrhoea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diarrhoea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">respiratory_infection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respiratory infection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">during_pregnancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During pregnancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">during_after_delivery__1_month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During/after delivery (&lt;1 month)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trauma_accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trauma/accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">violence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Violence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don_t_know</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t know</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other__specify_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vYsUPjPAfLpLZEGZqSvzbR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -496,11 +489,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -531,15 +523,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -821,29 +804,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="120" showGridLines="1" tabSelected="true">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="53.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="48.6640625" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="38" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="18.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="66.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="5.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="48.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="79.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="8.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="68.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="12.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="11.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -885,6 +868,7 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
+      <c r="D2"/>
       <c r="E2" t="s">
         <v>12</v>
       </c>
@@ -894,8 +878,11 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -905,11 +892,17 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -919,6 +912,7 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
+      <c r="D4"/>
       <c r="E4" t="s">
         <v>21</v>
       </c>
@@ -928,8 +922,11 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -939,14 +936,19 @@
       <c r="C5" t="s">
         <v>25</v>
       </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I5"/>
+      <c r="J5"/>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -956,14 +958,19 @@
       <c r="C6" t="s">
         <v>29</v>
       </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -973,11 +980,17 @@
       <c r="C7" t="s">
         <v>33</v>
       </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
       <c r="G7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -987,11 +1000,17 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
       <c r="G8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1001,6 +1020,7 @@
       <c r="C9" t="s">
         <v>38</v>
       </c>
+      <c r="D9"/>
       <c r="E9" t="s">
         <v>39</v>
       </c>
@@ -1013,8 +1033,10 @@
       <c r="H9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1024,14 +1046,19 @@
       <c r="C10" t="s">
         <v>43</v>
       </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
       <c r="G10" t="s">
         <v>14</v>
       </c>
       <c r="H10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I10"/>
+      <c r="J10"/>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1041,14 +1068,19 @@
       <c r="C11" t="s">
         <v>47</v>
       </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
       <c r="G11" t="s">
         <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1058,14 +1090,19 @@
       <c r="C12" t="s">
         <v>50</v>
       </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I12"/>
+      <c r="J12"/>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -1075,14 +1112,19 @@
       <c r="C13" t="s">
         <v>54</v>
       </c>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I13"/>
+      <c r="J13"/>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1107,8 +1149,10 @@
       <c r="H14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I14"/>
+      <c r="J14"/>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -1118,11 +1162,17 @@
       <c r="C15" t="s">
         <v>63</v>
       </c>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
       <c r="G15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1132,6 +1182,7 @@
       <c r="C16" t="s">
         <v>65</v>
       </c>
+      <c r="D16"/>
       <c r="E16" t="s">
         <v>66</v>
       </c>
@@ -1144,8 +1195,10 @@
       <c r="H16" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1155,11 +1208,17 @@
       <c r="C17" t="s">
         <v>71</v>
       </c>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
       <c r="G17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1169,6 +1228,7 @@
       <c r="C18" t="s">
         <v>73</v>
       </c>
+      <c r="D18"/>
       <c r="E18" t="s">
         <v>66</v>
       </c>
@@ -1181,8 +1241,10 @@
       <c r="H18" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -1192,11 +1254,17 @@
       <c r="C19" t="s">
         <v>77</v>
       </c>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
       <c r="G19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+    </row>
+    <row r="20">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1206,6 +1274,7 @@
       <c r="C20" t="s">
         <v>79</v>
       </c>
+      <c r="D20"/>
       <c r="E20" t="s">
         <v>66</v>
       </c>
@@ -1218,8 +1287,10 @@
       <c r="H20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20"/>
+      <c r="J20"/>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1229,11 +1300,17 @@
       <c r="C21" t="s">
         <v>83</v>
       </c>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
       <c r="G21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1243,6 +1320,7 @@
       <c r="C22" t="s">
         <v>85</v>
       </c>
+      <c r="D22"/>
       <c r="E22" t="s">
         <v>66</v>
       </c>
@@ -1255,8 +1333,10 @@
       <c r="H22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -1266,14 +1346,19 @@
       <c r="C23" t="s">
         <v>89</v>
       </c>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
       <c r="G23" t="s">
         <v>14</v>
       </c>
       <c r="H23" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23"/>
+      <c r="J23"/>
+    </row>
+    <row r="24">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1283,36 +1368,41 @@
       <c r="C24" t="s">
         <v>91</v>
       </c>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
       <c r="G24" t="s">
         <v>14</v>
       </c>
       <c r="H24" t="s">
         <v>92</v>
       </c>
+      <c r="I24"/>
+      <c r="J24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="120" showGridLines="1" tabSelected="false">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="30.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="51.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
@@ -1323,7 +1413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -1334,7 +1424,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1345,7 +1435,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1356,7 +1446,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -1367,7 +1457,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -1378,7 +1468,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -1389,7 +1479,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1400,7 +1490,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -1411,7 +1501,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -1422,7 +1512,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -1433,7 +1523,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -1444,7 +1534,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -1455,7 +1545,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -1466,7 +1556,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -1477,7 +1567,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -1488,7 +1578,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -1499,7 +1589,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -1510,7 +1600,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" t="s">
         <v>127</v>
       </c>
@@ -1521,7 +1611,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -1532,7 +1622,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -1543,7 +1633,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" t="s">
         <v>130</v>
       </c>
@@ -1554,7 +1644,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" t="s">
         <v>131</v>
       </c>
@@ -1565,7 +1655,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -1576,7 +1666,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -1587,7 +1677,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -1598,7 +1688,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1609,7 +1699,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1620,7 +1710,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -1631,7 +1721,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" t="s">
         <v>133</v>
       </c>
@@ -1642,7 +1732,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" t="s">
         <v>133</v>
       </c>
@@ -1653,7 +1743,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" t="s">
         <v>133</v>
       </c>
@@ -1664,7 +1754,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -1675,7 +1765,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -1686,7 +1776,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" t="s">
         <v>133</v>
       </c>
@@ -1697,7 +1787,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -1708,7 +1798,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -1721,36 +1811,36 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="120" showGridLines="1" tabSelected="false">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>